<commit_message>
Report and Output analysis
</commit_message>
<xml_diff>
--- a/Analysis/Cost_Analysis.xlsx
+++ b/Analysis/Cost_Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\INFO6205_FinalProject\INFO6205_FinalProject\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -272,11 +272,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="177275176"/>
-        <c:axId val="177272040"/>
+        <c:axId val="163663728"/>
+        <c:axId val="163657064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="177275176"/>
+        <c:axId val="163663728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -319,7 +319,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177272040"/>
+        <c:crossAx val="163657064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -327,10 +327,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177272040"/>
+        <c:axId val="163657064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="500000"/>
+          <c:min val="600000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -379,7 +379,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177275176"/>
+        <c:crossAx val="163663728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,7 +1272,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>